<commit_message>
Novo plano de aulas
</commit_message>
<xml_diff>
--- a/src/plano-de-aulas.xlsx
+++ b/src/plano-de-aulas.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="138">
   <si>
     <t xml:space="preserve">Data</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t xml:space="preserve">SEMANA AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primeiro problema de enumeração exaustiva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geração de cadeias de DNA. O tamanho dela é o parâmetro!</t>
   </si>
   <si>
     <t xml:space="preserve">Otimizar escolha de ativos levando em conta budget</t>
@@ -217,10 +223,7 @@
 "Algoritmo da mão direita": desenvolver método inicial para sair do labirinto e implementar.</t>
   </si>
   <si>
-    <t xml:space="preserve">Backtracking: outros problemas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Problemas de backtracking no leet-code ou algo similar</t>
+    <t xml:space="preserve">QUIZ NESSA SEMANA SOBRE RECURSÃO USANDO AULA CANCELADA!</t>
   </si>
   <si>
     <t xml:space="preserve">Como encontrar um caminho até o destino?</t>
@@ -308,21 +311,8 @@
     <t xml:space="preserve">Estruturas de Dados</t>
   </si>
   <si>
-    <t xml:space="preserve">Implementações de algoritmos com tipo lista
-Atividade: reimplementar algoritmos com diferentes tipos de lista </t>
-  </si>
-  <si>
     <t xml:space="preserve">Tipo Conjunto (array booleano)
 Atividade: reimplementar algoritmos com diferentes tipos de lista </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buscas consecutivas: Documento contém uma palavra?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expositiva: buscas consecutivas no mesmo texto
-Tipo Conjunto (array com elementos O(N)) + Tipo Dicionário
-Aluno constrói ambos tipos em cima do tipo Lista
-Complexidade Espaço vs Complexidade Tempo</t>
   </si>
   <si>
     <r>
@@ -411,6 +401,12 @@
 Implementação do algoritmo usando testes de unidade. Ref Skiena Cap 7</t>
   </si>
   <si>
+    <t xml:space="preserve">Backtracking: outros problemas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problemas de backtracking no leet-code ou algo similar</t>
+  </si>
+  <si>
     <t xml:space="preserve">Discussão: explorar problemas do algoritmo da aula passada
 Desenvolver algoritmo na lousa
 Aluno faz Implementação com testes de unidade
@@ -434,6 +430,13 @@
   </si>
   <si>
     <t xml:space="preserve">Ref Cormen cap 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementações de algoritmos com tipo lista
+Atividade: reimplementar algoritmos com diferentes tipos de lista </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscas consecutivas: Documento contém uma palavra?</t>
   </si>
   <si>
     <t xml:space="preserve">Expositiva: buscas consecutivas no mesmo texto
@@ -809,12 +812,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.5999"/>
-        <bgColor rgb="FFFFF2CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF5B277D"/>
         <bgColor rgb="FF3F3F76"/>
       </patternFill>
@@ -823,6 +820,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
         <bgColor rgb="FF9C0006"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.5999"/>
+        <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
     <fill>
@@ -931,15 +934,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -967,7 +970,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -979,7 +982,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -991,7 +994,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1003,19 +1006,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1023,23 +1014,35 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1047,7 +1050,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1059,7 +1062,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1339,10 +1342,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1356,7 +1359,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="24.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1540,7 +1543,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="1" t="n">
         <f aca="false">A8 + 7</f>
         <v>45908</v>
       </c>
@@ -1582,7 +1585,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <f aca="false">A10 + 7</f>
         <v>45915</v>
       </c>
@@ -1624,7 +1627,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="99.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <f aca="false">A12 + 7</f>
         <v>45922</v>
       </c>
@@ -1639,9 +1642,6 @@
         <v>36</v>
       </c>
       <c r="F14" s="15"/>
-      <c r="G14" s="0"/>
-      <c r="H14" s="0"/>
-      <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="93.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
@@ -1661,12 +1661,9 @@
         <v>36</v>
       </c>
       <c r="F15" s="15"/>
-      <c r="G15" s="0"/>
-      <c r="H15" s="0"/>
-      <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="106.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="16" t="n">
         <f aca="false">A14 + 7</f>
         <v>45929</v>
       </c>
@@ -1674,14 +1671,15 @@
       <c r="C16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="8"/>
+      <c r="E16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>39</v>
+      <c r="G16" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="138.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1691,7 +1689,7 @@
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>40</v>
@@ -1712,16 +1710,16 @@
         <v>11</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="121.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1732,30 +1730,17 @@
       <c r="B19" s="9" t="n">
         <v>12</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="5" t="s">
+      <c r="C19" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="139.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1767,29 +1752,19 @@
         <v>13</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="127.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1800,19 +1775,18 @@
       <c r="B21" s="9" t="n">
         <v>14</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="8" t="s">
+      <c r="C21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="n">
@@ -1823,29 +1797,16 @@
         <v>15</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="G22" s="0"/>
-      <c r="H22" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="202.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1856,30 +1817,20 @@
       <c r="B23" s="9" t="n">
         <v>16</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" s="0"/>
-      <c r="H23" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="I23" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="J23" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="K23" s="20" t="s">
-        <v>56</v>
+      <c r="G23" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="99.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1890,17 +1841,20 @@
       <c r="B24" s="9" t="n">
         <v>17</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>57</v>
+      <c r="C24" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="112.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1911,21 +1865,18 @@
       <c r="B25" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="0"/>
-      <c r="H25" s="0"/>
-      <c r="I25" s="0"/>
+      <c r="C25" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="167.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="n">
@@ -1935,15 +1886,12 @@
       <c r="B26" s="9" t="n">
         <v>19</v>
       </c>
-      <c r="C26" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="0"/>
-      <c r="H26" s="0"/>
-      <c r="I26" s="0"/>
+      <c r="C26" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="n">
@@ -1953,15 +1901,12 @@
       <c r="B27" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="C27" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="0"/>
-      <c r="H27" s="0"/>
-      <c r="I27" s="0"/>
+      <c r="C27" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
     </row>
     <row r="28" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="n">
@@ -1972,16 +1917,13 @@
         <v>21</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
-      <c r="G28" s="0"/>
-      <c r="H28" s="0"/>
-      <c r="I28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="16" t="n">
@@ -1992,16 +1934,13 @@
         <v>22</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
-      <c r="G29" s="0"/>
-      <c r="H29" s="0"/>
-      <c r="I29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="n">
@@ -2011,10 +1950,6 @@
       <c r="B30" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="C30" s="0"/>
-      <c r="D30" s="0"/>
-      <c r="E30" s="0"/>
-      <c r="F30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="16" t="n">
@@ -2024,10 +1959,6 @@
       <c r="B31" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C31" s="0"/>
-      <c r="D31" s="0"/>
-      <c r="E31" s="0"/>
-      <c r="F31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="n">
@@ -2035,21 +1966,13 @@
         <v>45985</v>
       </c>
       <c r="B32" s="15"/>
-      <c r="C32" s="0"/>
-      <c r="D32" s="0"/>
-      <c r="E32" s="0"/>
-      <c r="F32" s="0"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="n">
         <f aca="false">A31+7</f>
         <v>45987</v>
       </c>
       <c r="B33" s="15"/>
-      <c r="C33" s="0"/>
-      <c r="D33" s="0"/>
-      <c r="E33" s="0"/>
-      <c r="F33" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2071,10 +1994,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2088,7 +2011,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="24.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="25.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2111,10 +2034,8 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
         <v>45693</v>
       </c>
@@ -2133,10 +2054,8 @@
       <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="0"/>
-      <c r="I2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="54.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
         <v>45695</v>
       </c>
@@ -2155,10 +2074,8 @@
       <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="0"/>
-      <c r="I3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <f aca="false">A2+7</f>
         <v>45700</v>
@@ -2176,10 +2093,8 @@
       <c r="F4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="0"/>
-      <c r="I4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="132.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
         <f aca="false">A3+7</f>
         <v>45702</v>
@@ -2197,10 +2112,8 @@
       <c r="F5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="0"/>
-      <c r="I5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="132.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
         <f aca="false">A4+7</f>
         <v>45707</v>
@@ -2220,10 +2133,8 @@
       <c r="F6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="0"/>
-      <c r="I6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="93.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <f aca="false">A5+7</f>
         <v>45709</v>
@@ -2241,14 +2152,12 @@
         <v>8</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H7" s="0"/>
-      <c r="I7" s="0"/>
+        <v>58</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="s">
-        <v>61</v>
+      <c r="A8" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="5" t="s">
@@ -2257,8 +2166,6 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="H8" s="0"/>
-      <c r="I8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="81.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
@@ -2268,14 +2175,12 @@
       <c r="B9" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="H9" s="0"/>
-      <c r="I9" s="0"/>
+      <c r="C9" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
@@ -2285,12 +2190,10 @@
       <c r="B10" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="H10" s="0"/>
-      <c r="I10" s="0"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
     </row>
     <row r="11" customFormat="false" ht="65.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
@@ -2300,14 +2203,12 @@
       <c r="B11" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="H11" s="0"/>
-      <c r="I11" s="0"/>
+      <c r="C11" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="n">
@@ -2325,8 +2226,6 @@
       <c r="F12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="0"/>
-      <c r="I12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="99.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
@@ -2348,28 +2247,24 @@
       <c r="F13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="0"/>
-      <c r="I13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="99.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24" t="s">
-        <v>64</v>
+      <c r="A14" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H14" s="0"/>
-      <c r="I14" s="0"/>
+        <v>41</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="93.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
@@ -2380,19 +2275,17 @@
         <v>10</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" s="0"/>
-      <c r="I15" s="0"/>
+        <v>63</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
@@ -2401,17 +2294,15 @@
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="8" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8" t="s">
         <v>34</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" s="0"/>
-      <c r="I16" s="0"/>
+        <v>65</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="81.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
@@ -2431,8 +2322,6 @@
       <c r="F17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="0"/>
-      <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="103.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="n">
@@ -2452,8 +2341,6 @@
         <v>36</v>
       </c>
       <c r="F18" s="15"/>
-      <c r="H18" s="0"/>
-      <c r="I18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="n">
@@ -2473,8 +2360,6 @@
         <v>36</v>
       </c>
       <c r="F19" s="15"/>
-      <c r="H19" s="0"/>
-      <c r="I19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="n">
@@ -2494,8 +2379,6 @@
         <v>36</v>
       </c>
       <c r="F20" s="15"/>
-      <c r="H20" s="0"/>
-      <c r="I20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="n">
@@ -2506,19 +2389,17 @@
         <v>14</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E21" s="17" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" s="0"/>
-      <c r="I21" s="0"/>
+        <v>47</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="n">
@@ -2529,10 +2410,10 @@
         <v>15</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>8</v>
@@ -2540,8 +2421,6 @@
       <c r="F22" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H22" s="0"/>
-      <c r="I22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="112.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="n">
@@ -2552,10 +2431,10 @@
         <v>16</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E23" s="17" t="s">
         <v>8</v>
@@ -2563,8 +2442,6 @@
       <c r="F23" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H23" s="0"/>
-      <c r="I23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="99.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="n">
@@ -2575,10 +2452,10 @@
         <v>17</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E24" s="17" t="s">
         <v>8</v>
@@ -2586,8 +2463,6 @@
       <c r="F24" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H24" s="0"/>
-      <c r="I24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="112.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="n">
@@ -2598,7 +2473,7 @@
         <v>18</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>68</v>
@@ -2609,8 +2484,6 @@
       <c r="F25" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="0"/>
-      <c r="I25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="106.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="n">
@@ -2620,14 +2493,12 @@
       <c r="B26" s="9" t="n">
         <v>19</v>
       </c>
-      <c r="C26" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="H26" s="0"/>
-      <c r="I26" s="0"/>
+      <c r="C26" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
     </row>
     <row r="27" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="n">
@@ -2638,7 +2509,7 @@
         <v>20</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>68</v>
@@ -2649,8 +2520,6 @@
       <c r="F27" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H27" s="0"/>
-      <c r="I27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="n">
@@ -2661,7 +2530,7 @@
         <v>21</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>13</v>
@@ -2672,8 +2541,6 @@
       <c r="F28" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="0"/>
-      <c r="I28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="n">
@@ -2684,7 +2551,7 @@
         <v>22</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>13</v>
@@ -2693,10 +2560,8 @@
         <v>8</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H29" s="0"/>
-      <c r="I29" s="0"/>
+        <v>71</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="n">
@@ -2706,14 +2571,12 @@
       <c r="B30" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="C30" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="H30" s="0"/>
-      <c r="I30" s="0"/>
+      <c r="C30" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
     </row>
     <row r="31" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="n">
@@ -2723,20 +2586,18 @@
       <c r="B31" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C31" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="E31" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="H31" s="0"/>
-      <c r="I31" s="0"/>
+      <c r="C31" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="n">
@@ -2745,15 +2606,13 @@
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
-      <c r="H32" s="0"/>
-      <c r="I32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="n">
@@ -2762,15 +2621,13 @@
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E33" s="15"/>
       <c r="F33" s="15"/>
-      <c r="H33" s="0"/>
-      <c r="I33" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2796,7 +2653,7 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2856,7 +2713,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2962,7 +2819,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G7" s="26"/>
     </row>
@@ -3019,19 +2876,19 @@
         <v>8</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="99.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3043,19 +2900,19 @@
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3079,7 +2936,7 @@
         <v>26</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3089,17 +2946,17 @@
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="8" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8" t="s">
         <v>34</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="81.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3168,16 +3025,16 @@
         <v>13</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3189,10 +3046,10 @@
         <v>14</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>8</v>
@@ -3210,19 +3067,19 @@
         <v>15</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="112.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3234,16 +3091,16 @@
         <v>16</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="99.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3255,7 +3112,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>68</v>
@@ -3276,7 +3133,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>68</v>
@@ -3297,7 +3154,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>68</v>
@@ -3309,7 +3166,7 @@
         <v>69</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3321,16 +3178,16 @@
         <v>20</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E24" s="17" t="s">
         <v>8</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3342,7 +3199,7 @@
         <v>21</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>13</v>
@@ -3354,7 +3211,7 @@
         <v>70</v>
       </c>
       <c r="G25" s="30" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3366,7 +3223,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>13</v>
@@ -3375,10 +3232,10 @@
         <v>8</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="G26" s="30" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3390,19 +3247,19 @@
         <v>23</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G27" s="30" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3433,10 +3290,10 @@
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -3448,10 +3305,10 @@
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -3477,7 +3334,7 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -3512,13 +3369,13 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3568,13 +3425,13 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -3596,7 +3453,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3617,7 +3474,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3638,7 +3495,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3650,7 +3507,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>13</v>
@@ -3659,7 +3516,7 @@
         <v>8</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="155.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3671,7 +3528,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>13</v>
@@ -3680,7 +3537,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3692,16 +3549,16 @@
         <v>8</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="99.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3713,7 +3570,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>13</v>
@@ -3722,7 +3579,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3743,7 +3600,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3762,7 +3619,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="81.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3831,13 +3688,13 @@
         <v>13</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F17" s="7"/>
     </row>
@@ -3859,7 +3716,7 @@
         <v>8</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3874,13 +3731,13 @@
         <v>20</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3913,16 +3770,16 @@
         <v>17</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3934,16 +3791,16 @@
         <v>18</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3955,16 +3812,16 @@
         <v>19</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3976,7 +3833,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>68</v>
@@ -3985,7 +3842,7 @@
         <v>8</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3997,16 +3854,16 @@
         <v>21</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4018,13 +3875,13 @@
         <v>22</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F26" s="7"/>
     </row>
@@ -4037,16 +3894,16 @@
         <v>23</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4058,16 +3915,16 @@
         <v>24</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4077,10 +3934,10 @@
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -4092,10 +3949,10 @@
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -4121,7 +3978,7 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4156,13 +4013,13 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4212,13 +4069,13 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F4" s="7"/>
     </row>
@@ -4243,7 +4100,7 @@
         <v>11</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4258,13 +4115,13 @@
         <v>15</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4285,7 +4142,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4300,13 +4157,13 @@
         <v>15</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="155.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4318,7 +4175,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>13</v>
@@ -4327,7 +4184,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4339,7 +4196,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>13</v>
@@ -4348,7 +4205,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="88.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4360,16 +4217,16 @@
         <v>9</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4381,7 +4238,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>13</v>
@@ -4390,7 +4247,7 @@
         <v>8</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4409,7 +4266,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="81.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4428,10 +4285,10 @@
         <v>8</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="103.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4475,13 +4332,13 @@
         <v>12</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4493,13 +4350,13 @@
         <v>13</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F17" s="7"/>
     </row>
@@ -4521,7 +4378,7 @@
         <v>8</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4536,13 +4393,13 @@
         <v>20</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4575,16 +4432,16 @@
         <v>17</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4596,19 +4453,19 @@
         <v>18</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="G22" s="32" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4620,16 +4477,16 @@
         <v>19</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4641,7 +4498,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>68</v>
@@ -4650,7 +4507,7 @@
         <v>8</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4662,19 +4519,19 @@
         <v>21</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G25" s="32" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4686,13 +4543,13 @@
         <v>22</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F26" s="7"/>
     </row>
@@ -4705,16 +4562,16 @@
         <v>23</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4726,19 +4583,19 @@
         <v>24</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4748,10 +4605,10 @@
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
@@ -4763,10 +4620,10 @@
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
@@ -4792,7 +4649,7 @@
   </sheetPr>
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4824,13 +4681,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4881,7 +4738,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4893,13 +4750,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4908,7 +4765,7 @@
         <v>44979</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -4924,10 +4781,10 @@
       </c>
       <c r="C7" s="34"/>
       <c r="D7" s="8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="102" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4940,10 +4797,10 @@
       </c>
       <c r="C8" s="34"/>
       <c r="D8" s="8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="155.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4955,13 +4812,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4974,10 +4831,10 @@
       </c>
       <c r="C10" s="35"/>
       <c r="D10" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="88.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4995,7 +4852,7 @@
         <v>21</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5011,7 +4868,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5027,7 +4884,7 @@
         <v>30</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5036,7 +4893,7 @@
         <v>45007</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="37"/>
@@ -5048,7 +4905,7 @@
         <v>45009</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C15" s="37"/>
       <c r="D15" s="37"/>
@@ -5063,28 +4920,28 @@
         <v>12</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H16" s="4" t="n">
         <v>12</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="L16" s="33" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5100,7 +4957,7 @@
         <v>13</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5109,7 +4966,7 @@
         <v>45021</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -5121,7 +4978,7 @@
         <v>45023</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -5137,13 +4994,13 @@
       </c>
       <c r="C20" s="34"/>
       <c r="D20" s="8" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5155,13 +5012,13 @@
         <v>15</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5174,10 +5031,10 @@
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5186,7 +5043,7 @@
         <v>45037</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -5205,7 +5062,7 @@
         <v>68</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5218,10 +5075,10 @@
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5233,13 +5090,13 @@
         <v>19</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5253,7 +5110,7 @@
       <c r="C27" s="36"/>
       <c r="D27" s="9"/>
       <c r="E27" s="8" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5267,7 +5124,7 @@
       <c r="C28" s="36"/>
       <c r="D28" s="9"/>
       <c r="E28" s="8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5276,7 +5133,7 @@
         <v>45058</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>

</xml_diff>

<commit_message>
Aula 03 pronta -- handouts de strings!
</commit_message>
<xml_diff>
--- a/src/plano-de-aulas.xlsx
+++ b/src/plano-de-aulas.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="138">
   <si>
     <t xml:space="preserve">Data</t>
   </si>
@@ -140,6 +140,9 @@
 Discussão: algoritmo mergesort
 Implementações
 Ref Cormen cap 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUIZ NESSA SEMANA SOBRE RECURSÃO USANDO AULA CANCELADA!</t>
   </si>
   <si>
     <t xml:space="preserve">Revisão Geral</t>
@@ -221,9 +224,6 @@
   <si>
     <t xml:space="preserve">Representação do Labirinto usando Matriz
 "Algoritmo da mão direita": desenvolver método inicial para sair do labirinto e implementar.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QUIZ NESSA SEMANA SOBRE RECURSÃO USANDO AULA CANCELADA!</t>
   </si>
   <si>
     <t xml:space="preserve">Como encontrar um caminho até o destino?</t>
@@ -693,11 +693,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -929,7 +928,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -970,10 +969,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -994,10 +989,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1008,6 +999,10 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1344,11 +1339,11 @@
   </sheetPr>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
@@ -1506,17 +1501,17 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="n">
+      <c r="A8" s="3" t="n">
         <f aca="false">A6 + 7</f>
         <v>45901</v>
       </c>
       <c r="B8" s="9"/>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="81.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
@@ -1526,24 +1521,24 @@
       <c r="B9" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="11" t="s">
+      <c r="E9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="3" t="n">
         <f aca="false">A8 + 7</f>
         <v>45908</v>
       </c>
@@ -1585,7 +1580,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="3" t="n">
         <f aca="false">A10 + 7</f>
         <v>45915</v>
       </c>
@@ -1603,6 +1598,9 @@
       </c>
       <c r="F12" s="5" t="s">
         <v>31</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="99.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1614,34 +1612,34 @@
         <v>9</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="99.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="3" t="n">
         <f aca="false">A12 + 7</f>
         <v>45922</v>
       </c>
       <c r="B14" s="4"/>
-      <c r="C14" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="15"/>
+      <c r="C14" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="93.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
@@ -1651,34 +1649,34 @@
       <c r="B15" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="15"/>
+      <c r="C15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="106.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="n">
+      <c r="A16" s="3" t="n">
         <f aca="false">A14 + 7</f>
         <v>45929</v>
       </c>
-      <c r="B16" s="15"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="12" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1687,18 +1685,18 @@
         <f aca="false">A15+7</f>
         <v>45931</v>
       </c>
-      <c r="B17" s="15"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="134.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1710,20 +1708,20 @@
         <v>11</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="121.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="n">
+      <c r="A19" s="3" t="n">
         <f aca="false">A17 + 7</f>
         <v>45938</v>
       </c>
@@ -1731,16 +1729,16 @@
         <v>12</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="139.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1752,23 +1750,23 @@
         <v>13</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="127.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16" t="n">
+      <c r="A21" s="3" t="n">
         <f aca="false">A19 + 7</f>
         <v>45945</v>
       </c>
@@ -1776,7 +1774,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>49</v>
@@ -1796,13 +1794,13 @@
       <c r="B22" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>45</v>
+      <c r="C22" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="8" t="s">
@@ -1810,26 +1808,26 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="202.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16" t="n">
+      <c r="A23" s="3" t="n">
         <f aca="false">A21 + 7</f>
         <v>45952</v>
       </c>
       <c r="B23" s="9" t="n">
         <v>16</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>45</v>
+      <c r="C23" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="12" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1841,7 +1839,7 @@
       <c r="B24" s="9" t="n">
         <v>17</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="16" t="s">
         <v>53</v>
       </c>
       <c r="D24" s="6" t="s">
@@ -1853,25 +1851,25 @@
       <c r="F24" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="112.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16" t="n">
+      <c r="A25" s="3" t="n">
         <f aca="false">A23 + 7</f>
         <v>45959</v>
       </c>
       <c r="B25" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="C25" s="17" t="s">
-        <v>45</v>
+      <c r="C25" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="8" t="s">
@@ -1886,27 +1884,27 @@
       <c r="B26" s="9" t="n">
         <v>19</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
     </row>
     <row r="27" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="16" t="n">
+      <c r="A27" s="3" t="n">
         <f aca="false">A25 + 7</f>
         <v>45966</v>
       </c>
       <c r="B27" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
     </row>
     <row r="28" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="n">
@@ -1916,63 +1914,51 @@
       <c r="B28" s="9" t="n">
         <v>21</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
     </row>
     <row r="29" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="16" t="n">
+      <c r="A29" s="3" t="n">
         <f aca="false">A27 + 7</f>
         <v>45973</v>
       </c>
       <c r="B29" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
     </row>
     <row r="30" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="n">
-        <f aca="false">A28+7</f>
-        <v>45978</v>
-      </c>
+      <c r="A30" s="18"/>
       <c r="B30" s="4" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="16" t="n">
-        <f aca="false">A29 + 7</f>
-        <v>45980</v>
-      </c>
+      <c r="A31" s="3"/>
       <c r="B31" s="4" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="n">
-        <f aca="false">A30+7</f>
-        <v>45985</v>
-      </c>
-      <c r="B32" s="15"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="14"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="n">
-        <f aca="false">A31+7</f>
-        <v>45987</v>
-      </c>
-      <c r="B33" s="15"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2000,7 +1986,7 @@
       <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
@@ -2036,7 +2022,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="18" t="n">
         <v>45693</v>
       </c>
       <c r="B2" s="4" t="n">
@@ -2056,7 +2042,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="18" t="n">
         <v>45695</v>
       </c>
       <c r="B3" s="4" t="n">
@@ -2076,7 +2062,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="18" t="n">
         <f aca="false">A2+7</f>
         <v>45700</v>
       </c>
@@ -2095,7 +2081,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="18" t="n">
         <f aca="false">A3+7</f>
         <v>45702</v>
       </c>
@@ -2114,7 +2100,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="18" t="n">
         <f aca="false">A4+7</f>
         <v>45707</v>
       </c>
@@ -2135,7 +2121,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+      <c r="A7" s="18" t="n">
         <f aca="false">A5+7</f>
         <v>45709</v>
       </c>
@@ -2156,7 +2142,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="9"/>
@@ -2168,47 +2154,47 @@
       <c r="F8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="81.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+      <c r="A9" s="18" t="n">
         <f aca="false">A6+7</f>
         <v>45714</v>
       </c>
       <c r="B9" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+      <c r="A10" s="18" t="n">
         <f aca="false">A7+7</f>
         <v>45716</v>
       </c>
       <c r="B10" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" customFormat="false" ht="65.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+      <c r="A11" s="18" t="n">
         <f aca="false">A9+7</f>
         <v>45721</v>
       </c>
       <c r="B11" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
     </row>
     <row r="12" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="n">
@@ -2228,7 +2214,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="99.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+      <c r="A13" s="18" t="n">
         <f aca="false">A10+7</f>
         <v>45723</v>
       </c>
@@ -2249,25 +2235,25 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="99.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="20" t="s">
         <v>62</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="93.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+      <c r="A15" s="18" t="n">
         <f aca="false">A11+7</f>
         <v>45728</v>
       </c>
@@ -2275,10 +2261,10 @@
         <v>10</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>8</v>
@@ -2288,134 +2274,134 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+      <c r="A16" s="18" t="n">
         <f aca="false">A13+7</f>
         <v>45730</v>
       </c>
-      <c r="B16" s="15"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="8" t="s">
         <v>64</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="81.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+      <c r="A17" s="18" t="n">
         <f aca="false">A15+7</f>
         <v>45735</v>
       </c>
-      <c r="B17" s="15"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="103.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+      <c r="A18" s="18" t="n">
         <f aca="false">A16+7</f>
         <v>45737</v>
       </c>
       <c r="B18" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="15"/>
+      <c r="C18" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
+      <c r="A19" s="18" t="n">
         <f aca="false">A17+7</f>
         <v>45742</v>
       </c>
       <c r="B19" s="9" t="n">
         <v>12</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19" s="15"/>
+      <c r="C19" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
+      <c r="A20" s="18" t="n">
         <f aca="false">A18+7</f>
         <v>45744</v>
       </c>
       <c r="B20" s="9" t="n">
         <v>13</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="15"/>
+      <c r="C20" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="14"/>
     </row>
     <row r="21" customFormat="false" ht="106.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
+      <c r="A21" s="18" t="n">
         <f aca="false">A19+7</f>
         <v>45749</v>
       </c>
       <c r="B21" s="9" t="n">
         <v>14</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>45</v>
+      <c r="C21" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
+      <c r="A22" s="18" t="n">
         <f aca="false">A20+7</f>
         <v>45751</v>
       </c>
       <c r="B22" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>45</v>
+      <c r="C22" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="8" t="s">
@@ -2423,20 +2409,20 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="112.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
+      <c r="A23" s="18" t="n">
         <f aca="false">A21+7</f>
         <v>45756</v>
       </c>
       <c r="B23" s="9" t="n">
         <v>16</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>45</v>
+      <c r="C23" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F23" s="8" t="s">
@@ -2444,20 +2430,20 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="99.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
+      <c r="A24" s="18" t="n">
         <f aca="false">A22+7</f>
         <v>45758</v>
       </c>
       <c r="B24" s="9" t="n">
         <v>17</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>45</v>
+      <c r="C24" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -2465,20 +2451,20 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="112.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
+      <c r="A25" s="18" t="n">
         <f aca="false">A23+7</f>
         <v>45763</v>
       </c>
       <c r="B25" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="C25" s="17" t="s">
-        <v>45</v>
+      <c r="C25" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="8" t="s">
@@ -2486,35 +2472,35 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="106.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
+      <c r="A26" s="18" t="n">
         <f aca="false">A24+7</f>
         <v>45765</v>
       </c>
       <c r="B26" s="9" t="n">
         <v>19</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
     </row>
     <row r="27" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="n">
+      <c r="A27" s="18" t="n">
         <f aca="false">A25+7</f>
         <v>45770</v>
       </c>
       <c r="B27" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="C27" s="17" t="s">
-        <v>45</v>
+      <c r="C27" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F27" s="8" t="s">
@@ -2522,14 +2508,14 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="n">
+      <c r="A28" s="18" t="n">
         <f aca="false">A26+7</f>
         <v>45772</v>
       </c>
       <c r="B28" s="9" t="n">
         <v>21</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="16" t="s">
         <v>53</v>
       </c>
       <c r="D28" s="6" t="s">
@@ -2543,14 +2529,14 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="n">
+      <c r="A29" s="18" t="n">
         <f aca="false">A27+7</f>
         <v>45777</v>
       </c>
       <c r="B29" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="16" t="s">
         <v>53</v>
       </c>
       <c r="D29" s="6" t="s">
@@ -2564,70 +2550,70 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="n">
+      <c r="A30" s="18" t="n">
         <f aca="false">A28+7</f>
         <v>45779</v>
       </c>
       <c r="B30" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
     </row>
     <row r="31" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="n">
+      <c r="A31" s="18" t="n">
         <f aca="false">A29+7</f>
         <v>45784</v>
       </c>
       <c r="B31" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="D31" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="24" t="s">
+      <c r="E31" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="23" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="n">
+      <c r="A32" s="18" t="n">
         <f aca="false">A30+7</f>
         <v>45786</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="14" t="s">
+      <c r="B32" s="14"/>
+      <c r="C32" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="n">
+      <c r="A33" s="18" t="n">
         <f aca="false">A31+7</f>
         <v>45791</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="14" t="s">
+      <c r="B33" s="14"/>
+      <c r="C33" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2657,7 +2643,7 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
@@ -2694,7 +2680,7 @@
       <c r="I1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="18" t="n">
         <v>45511</v>
       </c>
       <c r="B2" s="4" t="n">
@@ -2712,12 +2698,12 @@
       <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="18" t="n">
         <v>45513</v>
       </c>
       <c r="B3" s="4" t="n">
@@ -2735,10 +2721,10 @@
       <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="26"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="18" t="n">
         <f aca="false">A2+7</f>
         <v>45518</v>
       </c>
@@ -2755,10 +2741,10 @@
       <c r="F4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="26"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="18" t="n">
         <f aca="false">A3+7</f>
         <v>45520</v>
       </c>
@@ -2777,10 +2763,10 @@
       <c r="F5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="26"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="18" t="n">
         <f aca="false">A4+7</f>
         <v>45525</v>
       </c>
@@ -2799,10 +2785,10 @@
       <c r="F6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+      <c r="A7" s="18" t="n">
         <f aca="false">A5+7</f>
         <v>45527</v>
       </c>
@@ -2821,10 +2807,10 @@
       <c r="F7" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="26"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+      <c r="A8" s="18" t="n">
         <f aca="false">A6+7</f>
         <v>45532</v>
       </c>
@@ -2843,10 +2829,10 @@
       <c r="F8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="25"/>
     </row>
     <row r="9" customFormat="false" ht="65.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+      <c r="A9" s="18" t="n">
         <f aca="false">A7+7</f>
         <v>45534</v>
       </c>
@@ -2865,10 +2851,10 @@
       <c r="F9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="26"/>
+      <c r="G9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+      <c r="A10" s="18" t="n">
         <f aca="false">A8+7</f>
         <v>45539</v>
       </c>
@@ -2876,23 +2862,23 @@
         <v>8</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="26" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="99.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+      <c r="A11" s="18" t="n">
         <f aca="false">A9+7</f>
         <v>45541</v>
       </c>
@@ -2900,10 +2886,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>8</v>
@@ -2911,12 +2897,12 @@
       <c r="F11" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="27" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+      <c r="A12" s="18" t="n">
         <f aca="false">A10+7</f>
         <v>45546</v>
       </c>
@@ -2935,123 +2921,123 @@
       <c r="F12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="27" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+      <c r="A13" s="18" t="n">
         <f aca="false">A11+7</f>
         <v>45548</v>
       </c>
-      <c r="B13" s="15"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="8" t="s">
         <v>64</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="28" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="81.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+      <c r="A14" s="18" t="n">
         <f aca="false">A12+7</f>
         <v>45553</v>
       </c>
-      <c r="B14" s="15"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="103.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+      <c r="A15" s="18" t="n">
         <f aca="false">A13+7</f>
         <v>45555</v>
       </c>
       <c r="B15" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="15"/>
+      <c r="C15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+      <c r="A16" s="18" t="n">
         <f aca="false">A14+7</f>
         <v>45560</v>
       </c>
       <c r="B16" s="9" t="n">
         <v>12</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="15"/>
+      <c r="C16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+      <c r="A17" s="18" t="n">
         <f aca="false">A15+7</f>
         <v>45562</v>
       </c>
       <c r="B17" s="9" t="n">
         <v>13</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>45</v>
+      <c r="C17" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+      <c r="A18" s="18" t="n">
         <f aca="false">A16+7</f>
         <v>45567</v>
       </c>
       <c r="B18" s="9" t="n">
         <v>14</v>
       </c>
-      <c r="C18" s="17" t="s">
-        <v>45</v>
+      <c r="C18" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="8" t="s">
@@ -3059,44 +3045,44 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
+      <c r="A19" s="18" t="n">
         <f aca="false">A17+7</f>
         <v>45569</v>
       </c>
       <c r="B19" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>45</v>
+      <c r="C19" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G19" s="27" t="s">
+      <c r="G19" s="26" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="112.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
+      <c r="A20" s="18" t="n">
         <f aca="false">A18+7</f>
         <v>45574</v>
       </c>
       <c r="B20" s="9" t="n">
         <v>16</v>
       </c>
-      <c r="C20" s="17" t="s">
-        <v>45</v>
+      <c r="C20" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="8" t="s">
@@ -3104,20 +3090,20 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="99.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
+      <c r="A21" s="18" t="n">
         <f aca="false">A19+7</f>
         <v>45576</v>
       </c>
       <c r="B21" s="9" t="n">
         <v>17</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>45</v>
+      <c r="C21" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="8" t="s">
@@ -3125,20 +3111,20 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="112.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
+      <c r="A22" s="18" t="n">
         <f aca="false">A20+7</f>
         <v>45581</v>
       </c>
       <c r="B22" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>45</v>
+      <c r="C22" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="8" t="s">
@@ -3146,44 +3132,44 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="106.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
+      <c r="A23" s="18" t="n">
         <f aca="false">A21+7</f>
         <v>45583</v>
       </c>
       <c r="B23" s="9" t="n">
         <v>19</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>45</v>
+      <c r="C23" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="G23" s="27" t="s">
+      <c r="G23" s="26" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
+      <c r="A24" s="18" t="n">
         <f aca="false">A22+7</f>
         <v>45588</v>
       </c>
       <c r="B24" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>45</v>
+      <c r="C24" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="E24" s="15" t="s">
         <v>8</v>
       </c>
       <c r="F24" s="8" t="s">
@@ -3191,14 +3177,14 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
+      <c r="A25" s="18" t="n">
         <f aca="false">A23+7</f>
         <v>45590</v>
       </c>
       <c r="B25" s="9" t="n">
         <v>21</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="16" t="s">
         <v>53</v>
       </c>
       <c r="D25" s="6" t="s">
@@ -3210,19 +3196,19 @@
       <c r="F25" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G25" s="30" t="s">
+      <c r="G25" s="29" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
+      <c r="A26" s="18" t="n">
         <f aca="false">A24+7</f>
         <v>45595</v>
       </c>
       <c r="B26" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="16" t="s">
         <v>53</v>
       </c>
       <c r="D26" s="6" t="s">
@@ -3234,19 +3220,19 @@
       <c r="F26" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G26" s="30" t="s">
+      <c r="G26" s="29" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="n">
+      <c r="A27" s="18" t="n">
         <f aca="false">A25+7</f>
         <v>45597</v>
       </c>
       <c r="B27" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="16" t="s">
         <v>53</v>
       </c>
       <c r="D27" s="6" t="s">
@@ -3258,60 +3244,60 @@
       <c r="F27" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G27" s="30" t="s">
+      <c r="G27" s="29" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="n">
+      <c r="A28" s="18" t="n">
         <f aca="false">A26+7</f>
         <v>45602</v>
       </c>
       <c r="B28" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>32</v>
+      <c r="C28" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="17" t="s">
         <v>34</v>
       </c>
+      <c r="E28" s="15" t="s">
+        <v>35</v>
+      </c>
       <c r="F28" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="n">
+      <c r="A29" s="18" t="n">
         <f aca="false">A27+7</f>
         <v>45604</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="14" t="s">
+      <c r="B29" s="14"/>
+      <c r="C29" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="n">
+      <c r="A30" s="18" t="n">
         <f aca="false">A28+7</f>
         <v>45609</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="14" t="s">
+      <c r="B30" s="14"/>
+      <c r="C30" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3338,7 +3324,7 @@
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
@@ -3379,7 +3365,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="18" t="n">
         <v>45329</v>
       </c>
       <c r="B2" s="4" t="n">
@@ -3399,7 +3385,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="18" t="n">
         <v>45331</v>
       </c>
       <c r="B3" s="4" t="n">
@@ -3419,7 +3405,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="18" t="n">
         <f aca="false">A2+7</f>
         <v>45336</v>
       </c>
@@ -3430,20 +3416,20 @@
       <c r="D4" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="30" t="s">
         <v>87</v>
       </c>
       <c r="F4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="18" t="n">
         <f aca="false">A3+7</f>
         <v>45338</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -3457,14 +3443,14 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="18" t="n">
         <f aca="false">A4+7</f>
         <v>45343</v>
       </c>
       <c r="B6" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="15" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -3478,14 +3464,14 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="122.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+      <c r="A7" s="18" t="n">
         <f aca="false">A5+7</f>
         <v>45345</v>
       </c>
       <c r="B7" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="15" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -3499,14 +3485,14 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+      <c r="A8" s="18" t="n">
         <f aca="false">A6+7</f>
         <v>45350</v>
       </c>
       <c r="B8" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="16" t="s">
         <v>53</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -3520,14 +3506,14 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="155.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+      <c r="A9" s="18" t="n">
         <f aca="false">A7+7</f>
         <v>45352</v>
       </c>
       <c r="B9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="16" t="s">
         <v>53</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -3541,14 +3527,14 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+      <c r="A10" s="18" t="n">
         <f aca="false">A8+7</f>
         <v>45357</v>
       </c>
       <c r="B10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="16" t="s">
         <v>53</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -3562,7 +3548,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="99.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+      <c r="A11" s="18" t="n">
         <f aca="false">A9+7</f>
         <v>45359</v>
       </c>
@@ -3583,14 +3569,14 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+      <c r="A12" s="18" t="n">
         <f aca="false">A10+7</f>
         <v>45364</v>
       </c>
       <c r="B12" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="8" t="s">
@@ -3604,12 +3590,12 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+      <c r="A13" s="18" t="n">
         <f aca="false">A11+7</f>
         <v>45366</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="17" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="8" t="s">
@@ -3623,64 +3609,64 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="81.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+      <c r="A14" s="18" t="n">
         <f aca="false">A12+7</f>
         <v>45371</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="17" t="s">
-        <v>32</v>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="103.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+      <c r="A15" s="18" t="n">
         <f aca="false">A13+7</f>
         <v>45373</v>
       </c>
       <c r="B15" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="15"/>
+      <c r="C15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+      <c r="A16" s="18" t="n">
         <f aca="false">A14+7</f>
         <v>45378</v>
       </c>
       <c r="B16" s="9" t="n">
         <v>12</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="15"/>
+      <c r="C16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+      <c r="A17" s="18" t="n">
         <f aca="false">A15+7</f>
         <v>45380</v>
       </c>
@@ -3693,20 +3679,20 @@
       <c r="D17" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="30" t="s">
         <v>87</v>
       </c>
       <c r="F17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+      <c r="A18" s="18" t="n">
         <f aca="false">A16+7</f>
         <v>45385</v>
       </c>
       <c r="B18" s="9" t="n">
         <v>14</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="8" t="s">
@@ -3720,14 +3706,14 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
+      <c r="A19" s="18" t="n">
         <f aca="false">A17+7</f>
         <v>45387</v>
       </c>
       <c r="B19" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="8" t="s">
@@ -3741,7 +3727,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
+      <c r="A20" s="18" t="n">
         <f aca="false">A18+7</f>
         <v>45392</v>
       </c>
@@ -3762,36 +3748,36 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
+      <c r="A21" s="18" t="n">
         <f aca="false">A19+7</f>
         <v>45394</v>
       </c>
       <c r="B21" s="9" t="n">
         <v>17</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>45</v>
+      <c r="C21" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
+      <c r="A22" s="18" t="n">
         <f aca="false">A20+7</f>
         <v>45399</v>
       </c>
       <c r="B22" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>45</v>
+      <c r="C22" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>49</v>
@@ -3804,15 +3790,15 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
+      <c r="A23" s="18" t="n">
         <f aca="false">A21+7</f>
         <v>45401</v>
       </c>
       <c r="B23" s="9" t="n">
         <v>19</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>45</v>
+      <c r="C23" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>81</v>
@@ -3825,15 +3811,15 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
+      <c r="A24" s="18" t="n">
         <f aca="false">A22+7</f>
         <v>45406</v>
       </c>
       <c r="B24" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>45</v>
+      <c r="C24" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>68</v>
@@ -3846,15 +3832,15 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
+      <c r="A25" s="18" t="n">
         <f aca="false">A23+7</f>
         <v>45408</v>
       </c>
       <c r="B25" s="9" t="n">
         <v>21</v>
       </c>
-      <c r="C25" s="17" t="s">
-        <v>45</v>
+      <c r="C25" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>81</v>
@@ -3867,7 +3853,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
+      <c r="A26" s="18" t="n">
         <f aca="false">A24+7</f>
         <v>45413</v>
       </c>
@@ -3880,24 +3866,24 @@
       <c r="D26" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="31" t="s">
+      <c r="E26" s="30" t="s">
         <v>87</v>
       </c>
       <c r="F26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="n">
+      <c r="A27" s="18" t="n">
         <f aca="false">A25+7</f>
         <v>45415</v>
       </c>
       <c r="B27" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="C27" s="18" t="s">
-        <v>39</v>
+      <c r="C27" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>8</v>
@@ -3907,18 +3893,18 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="n">
+      <c r="A28" s="18" t="n">
         <f aca="false">A26+7</f>
         <v>45420</v>
       </c>
       <c r="B28" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C28" s="18" t="s">
-        <v>39</v>
+      <c r="C28" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>8</v>
@@ -3928,34 +3914,34 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="n">
+      <c r="A29" s="18" t="n">
         <f aca="false">A27+7</f>
         <v>45422</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="14" t="s">
+      <c r="B29" s="14"/>
+      <c r="C29" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="n">
+      <c r="A30" s="18" t="n">
         <f aca="false">A28+7</f>
         <v>45427</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="14" t="s">
+      <c r="B30" s="14"/>
+      <c r="C30" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3982,7 +3968,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
@@ -4023,7 +4009,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="18" t="n">
         <v>45329</v>
       </c>
       <c r="B2" s="4" t="n">
@@ -4043,7 +4029,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="18" t="n">
         <v>45331</v>
       </c>
       <c r="B3" s="4" t="n">
@@ -4063,7 +4049,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="18" t="n">
         <f aca="false">A2+7</f>
         <v>45336</v>
       </c>
@@ -4074,13 +4060,13 @@
       <c r="D4" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="30" t="s">
         <v>87</v>
       </c>
       <c r="F4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="18" t="n">
         <f aca="false">A3+7</f>
         <v>45338</v>
       </c>
@@ -4099,19 +4085,19 @@
       <c r="F5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="31" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="18" t="n">
         <f aca="false">A4+7</f>
         <v>45343</v>
       </c>
       <c r="B6" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="15" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -4125,14 +4111,14 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+      <c r="A7" s="18" t="n">
         <f aca="false">A5+7</f>
         <v>45345</v>
       </c>
       <c r="B7" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="15" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -4146,14 +4132,14 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+      <c r="A8" s="18" t="n">
         <f aca="false">A6+7</f>
         <v>45350</v>
       </c>
       <c r="B8" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="15" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -4167,14 +4153,14 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="155.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+      <c r="A9" s="18" t="n">
         <f aca="false">A7+7</f>
         <v>45352</v>
       </c>
       <c r="B9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="16" t="s">
         <v>109</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -4188,14 +4174,14 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+      <c r="A10" s="18" t="n">
         <f aca="false">A8+7</f>
         <v>45357</v>
       </c>
       <c r="B10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="16" t="s">
         <v>109</v>
       </c>
       <c r="D10" s="6" t="s">
@@ -4209,14 +4195,14 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="88.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+      <c r="A11" s="18" t="n">
         <f aca="false">A9+7</f>
         <v>45359</v>
       </c>
       <c r="B11" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="16" t="s">
         <v>109</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -4230,7 +4216,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+      <c r="A12" s="18" t="n">
         <f aca="false">A10+7</f>
         <v>45364</v>
       </c>
@@ -4251,12 +4237,12 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+      <c r="A13" s="18" t="n">
         <f aca="false">A11+7</f>
         <v>45366</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="17" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="8" t="s">
@@ -4270,12 +4256,12 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="81.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+      <c r="A14" s="18" t="n">
         <f aca="false">A12+7</f>
         <v>45371</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="17" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="8" t="s">
@@ -4292,46 +4278,46 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="103.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+      <c r="A15" s="18" t="n">
         <f aca="false">A13+7</f>
         <v>45373</v>
       </c>
       <c r="B15" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="15"/>
+      <c r="C15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+      <c r="A16" s="18" t="n">
         <f aca="false">A14+7</f>
         <v>45378</v>
       </c>
       <c r="B16" s="9" t="n">
         <v>12</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="15"/>
+      <c r="C16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="14"/>
       <c r="I16" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="J16" s="18" t="s">
+      <c r="J16" s="16" t="s">
         <v>115</v>
       </c>
       <c r="K16" s="5" t="s">
@@ -4342,7 +4328,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+      <c r="A17" s="18" t="n">
         <f aca="false">A15+7</f>
         <v>45380</v>
       </c>
@@ -4355,20 +4341,20 @@
       <c r="D17" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="30" t="s">
         <v>87</v>
       </c>
       <c r="F17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+      <c r="A18" s="18" t="n">
         <f aca="false">A16+7</f>
         <v>45385</v>
       </c>
       <c r="B18" s="9" t="n">
         <v>14</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="8" t="s">
@@ -4382,14 +4368,14 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
+      <c r="A19" s="18" t="n">
         <f aca="false">A17+7</f>
         <v>45387</v>
       </c>
       <c r="B19" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="15" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="8" t="s">
@@ -4403,7 +4389,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
+      <c r="A20" s="18" t="n">
         <f aca="false">A18+7</f>
         <v>45392</v>
       </c>
@@ -4424,36 +4410,36 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
+      <c r="A21" s="18" t="n">
         <f aca="false">A19+7</f>
         <v>45394</v>
       </c>
       <c r="B21" s="9" t="n">
         <v>17</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>45</v>
+      <c r="C21" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
+      <c r="A22" s="18" t="n">
         <f aca="false">A20+7</f>
         <v>45399</v>
       </c>
       <c r="B22" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>45</v>
+      <c r="C22" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>49</v>
@@ -4464,20 +4450,20 @@
       <c r="F22" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="G22" s="31" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
+      <c r="A23" s="18" t="n">
         <f aca="false">A21+7</f>
         <v>45401</v>
       </c>
       <c r="B23" s="9" t="n">
         <v>19</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>45</v>
+      <c r="C23" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>81</v>
@@ -4490,15 +4476,15 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
+      <c r="A24" s="18" t="n">
         <f aca="false">A22+7</f>
         <v>45406</v>
       </c>
       <c r="B24" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>45</v>
+      <c r="C24" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>68</v>
@@ -4511,15 +4497,15 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
+      <c r="A25" s="18" t="n">
         <f aca="false">A23+7</f>
         <v>45408</v>
       </c>
       <c r="B25" s="9" t="n">
         <v>21</v>
       </c>
-      <c r="C25" s="17" t="s">
-        <v>45</v>
+      <c r="C25" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>81</v>
@@ -4530,12 +4516,12 @@
       <c r="F25" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G25" s="32" t="s">
+      <c r="G25" s="31" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
+      <c r="A26" s="18" t="n">
         <f aca="false">A24+7</f>
         <v>45413</v>
       </c>
@@ -4548,24 +4534,24 @@
       <c r="D26" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="31" t="s">
+      <c r="E26" s="30" t="s">
         <v>87</v>
       </c>
       <c r="F26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="n">
+      <c r="A27" s="18" t="n">
         <f aca="false">A25+7</f>
         <v>45415</v>
       </c>
       <c r="B27" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="C27" s="18" t="s">
-        <v>39</v>
+      <c r="C27" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>8</v>
@@ -4575,18 +4561,18 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="n">
+      <c r="A28" s="18" t="n">
         <f aca="false">A26+7</f>
         <v>45420</v>
       </c>
       <c r="B28" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C28" s="18" t="s">
-        <v>39</v>
+      <c r="C28" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>8</v>
@@ -4594,39 +4580,39 @@
       <c r="F28" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="G28" s="32" t="s">
+      <c r="G28" s="31" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="n">
+      <c r="A29" s="18" t="n">
         <f aca="false">A27+7</f>
         <v>45422</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="14" t="s">
+      <c r="B29" s="14"/>
+      <c r="C29" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="n">
+      <c r="A30" s="18" t="n">
         <f aca="false">A28+7</f>
         <v>45427</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="14" t="s">
+      <c r="B30" s="14"/>
+      <c r="C30" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4653,7 +4639,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.86"/>
@@ -4691,7 +4677,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="18" t="n">
         <v>44965</v>
       </c>
       <c r="B2" s="4" t="n">
@@ -4708,7 +4694,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="18" t="n">
         <v>44967</v>
       </c>
       <c r="B3" s="4" t="n">
@@ -4723,7 +4709,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="18" t="n">
         <f aca="false">A2+7</f>
         <v>44972</v>
       </c>
@@ -4737,19 +4723,19 @@
       <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="32" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="18" t="n">
         <f aca="false">A3+7</f>
         <v>44974</v>
       </c>
       <c r="B5" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="33" t="s">
         <v>120</v>
       </c>
       <c r="D5" s="8" t="s">
@@ -4760,7 +4746,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="18" t="n">
         <f aca="false">A4+7</f>
         <v>44979</v>
       </c>
@@ -4772,14 +4758,14 @@
       <c r="E6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="n">
+      <c r="A7" s="18" t="n">
         <f aca="false">A5+7</f>
         <v>44981</v>
       </c>
       <c r="B7" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="34"/>
+      <c r="C7" s="33"/>
       <c r="D7" s="8" t="s">
         <v>122</v>
       </c>
@@ -4788,14 +4774,14 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="102" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="n">
+      <c r="A8" s="18" t="n">
         <f aca="false">A6+7</f>
         <v>44986</v>
       </c>
       <c r="B8" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="34"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="8" t="s">
         <v>124</v>
       </c>
@@ -4804,14 +4790,14 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="155.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="n">
+      <c r="A9" s="18" t="n">
         <f aca="false">A7+7</f>
         <v>44988</v>
       </c>
       <c r="B9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="34" t="s">
         <v>126</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -4822,14 +4808,14 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
+      <c r="A10" s="18" t="n">
         <f aca="false">A8+7</f>
         <v>44993</v>
       </c>
       <c r="B10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="35"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="5" t="s">
         <v>128</v>
       </c>
@@ -4838,14 +4824,14 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="88.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
+      <c r="A11" s="18" t="n">
         <f aca="false">A9+7</f>
         <v>44995</v>
       </c>
       <c r="B11" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="35" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="8" t="s">
@@ -4856,14 +4842,14 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="n">
+      <c r="A12" s="18" t="n">
         <f aca="false">A10+7</f>
         <v>45000</v>
       </c>
       <c r="B12" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="C12" s="36"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="8" t="s">
         <v>28</v>
       </c>
@@ -4872,14 +4858,14 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="n">
+      <c r="A13" s="18" t="n">
         <f aca="false">A11+7</f>
         <v>45002</v>
       </c>
       <c r="B13" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="C13" s="36"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="8" t="s">
         <v>30</v>
       </c>
@@ -4888,38 +4874,38 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="n">
+      <c r="A14" s="18" t="n">
         <f aca="false">A12+7</f>
         <v>45007</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
     </row>
     <row r="15" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
+      <c r="A15" s="18" t="n">
         <f aca="false">A13+7</f>
         <v>45009</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
     </row>
     <row r="16" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
+      <c r="A16" s="18" t="n">
         <f aca="false">A14+7</f>
         <v>45014</v>
       </c>
       <c r="B16" s="9" t="n">
         <v>12</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="33" t="s">
         <v>109</v>
       </c>
       <c r="D16" s="8" t="s">
@@ -4931,7 +4917,7 @@
       <c r="H16" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="I16" s="16" t="s">
         <v>115</v>
       </c>
       <c r="J16" s="5" t="s">
@@ -4940,28 +4926,28 @@
       <c r="K16" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="L16" s="33" t="s">
+      <c r="L16" s="32" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
+      <c r="A17" s="18" t="n">
         <f aca="false">A15+7</f>
         <v>45016</v>
       </c>
       <c r="B17" s="9" t="n">
         <v>13</v>
       </c>
-      <c r="C17" s="34"/>
+      <c r="C17" s="33"/>
       <c r="D17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="38" t="s">
+      <c r="E17" s="37" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
+      <c r="A18" s="18" t="n">
         <f aca="false">A16+7</f>
         <v>45021</v>
       </c>
@@ -4973,7 +4959,7 @@
       <c r="E18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
+      <c r="A19" s="18" t="n">
         <f aca="false">A17+7</f>
         <v>45023</v>
       </c>
@@ -4985,26 +4971,26 @@
       <c r="E19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
+      <c r="A20" s="18" t="n">
         <f aca="false">A18+7</f>
         <v>45028</v>
       </c>
       <c r="B20" s="9" t="n">
         <v>14</v>
       </c>
-      <c r="C20" s="34"/>
+      <c r="C20" s="33"/>
       <c r="D20" s="8" t="s">
         <v>72</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="32" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
+      <c r="A21" s="18" t="n">
         <f aca="false">A19+7</f>
         <v>45030</v>
       </c>
@@ -5015,14 +5001,14 @@
         <v>132</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
+      <c r="A22" s="18" t="n">
         <f aca="false">A20+7</f>
         <v>45035</v>
       </c>
@@ -5038,7 +5024,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
+      <c r="A23" s="18" t="n">
         <f aca="false">A21+7</f>
         <v>45037</v>
       </c>
@@ -5050,7 +5036,7 @@
       <c r="E23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
+      <c r="A24" s="18" t="n">
         <f aca="false">A22+7</f>
         <v>45042</v>
       </c>
@@ -5066,7 +5052,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
+      <c r="A25" s="18" t="n">
         <f aca="false">A23+7</f>
         <v>45044</v>
       </c>
@@ -5082,83 +5068,83 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="n">
+      <c r="A26" s="18" t="n">
         <f aca="false">A24+7</f>
         <v>45049</v>
       </c>
       <c r="B26" s="9" t="n">
         <v>19</v>
       </c>
-      <c r="C26" s="36" t="s">
+      <c r="C26" s="35" t="s">
         <v>136</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="n">
+      <c r="A27" s="18" t="n">
         <f aca="false">A25+7</f>
         <v>45051</v>
       </c>
       <c r="B27" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="C27" s="36"/>
+      <c r="C27" s="35"/>
       <c r="D27" s="9"/>
       <c r="E27" s="8" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="n">
+      <c r="A28" s="18" t="n">
         <f aca="false">A26+7</f>
         <v>45056</v>
       </c>
       <c r="B28" s="9" t="n">
         <v>21</v>
       </c>
-      <c r="C28" s="36"/>
+      <c r="C28" s="35"/>
       <c r="D28" s="9"/>
       <c r="E28" s="8" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="n">
+      <c r="A29" s="18" t="n">
         <f aca="false">A27+7</f>
         <v>45058</v>
       </c>
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="n">
+      <c r="A30" s="18" t="n">
         <f aca="false">A28+7</f>
         <v>45063</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="n">
+      <c r="A31" s="18" t="n">
         <f aca="false">A29+7</f>
         <v>45065</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="n">
+      <c r="A32" s="18" t="n">
         <f aca="false">A30+7</f>
         <v>45070</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="n">
+      <c r="A33" s="18" t="n">
         <f aca="false">A31+7</f>
         <v>45072</v>
       </c>

</xml_diff>